<commit_message>
penambahan kolom nik untuk user
</commit_message>
<xml_diff>
--- a/public/assets/template/pic_template.xlsx
+++ b/public/assets/template/pic_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aryaw\Documents\BIlly\template excel gps_hrms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\gps_monitoring\public\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE6B32A-6EE0-4137-8182-3BD55A87FF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CF4278-AB36-49DF-8155-A041D8293987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>Catatan</t>
   </si>
   <si>
-    <t>Pastikan format email benar</t>
-  </si>
-  <si>
     <t>Pastikan role di isi dengan ID dari sheet Role</t>
   </si>
   <si>
@@ -108,19 +105,22 @@
     <t>department</t>
   </si>
   <si>
-    <t>andrian@globalpromedika.co.id</t>
-  </si>
-  <si>
     <t>Dwiari</t>
   </si>
   <si>
     <t>Rahmadi</t>
   </si>
   <si>
-    <t>billy@globalpromedika.co.id</t>
-  </si>
-  <si>
     <t>2050-09-01</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>nik</t>
+  </si>
+  <si>
+    <t>Pastikan format nik dan phone benar</t>
   </si>
 </sst>
 </file>
@@ -326,47 +326,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -760,24 +760,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -791,7 +794,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -803,80 +806,80 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="17" t="s">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -884,82 +887,91 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
+      <c r="C15" s="7">
+        <v>321616</v>
+      </c>
+      <c r="D15" s="7">
+        <v>857777</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
       </c>
-      <c r="G15" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="7">
+        <v>321717</v>
+      </c>
+      <c r="D16" s="7">
+        <v>12345678</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -967,25 +979,28 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="F19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" s="5"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -1000,12 +1015,14 @@
     <mergeCell ref="A9:H9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" xr:uid="{5B90E633-800B-4A1C-BE30-8F1DEAD89469}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{88925AA8-28F0-421E-AF16-7C87C2F2AFCA}"/>
+    <hyperlink ref="C15" r:id="rId1" display="andrian@globalpromedika.co.id" xr:uid="{5B90E633-800B-4A1C-BE30-8F1DEAD89469}"/>
+    <hyperlink ref="C16" r:id="rId2" display="billy@globalpromedika.co.id" xr:uid="{88925AA8-28F0-421E-AF16-7C87C2F2AFCA}"/>
+    <hyperlink ref="D15" r:id="rId3" display="andrian@globalpromedika.co.id" xr:uid="{40D56AA3-3D08-4D88-A4D7-5CB91405A7FB}"/>
+    <hyperlink ref="D16" r:id="rId4" display="billy@globalpromedika.co.id" xr:uid="{A567A305-5E20-4472-B501-CDD0FE359E78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1017,12 +1034,12 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1030,28 +1047,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1067,12 +1084,12 @@
       <selection activeCell="C6" sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1080,7 +1097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1088,7 +1105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1096,7 +1113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>

</xml_diff>